<commit_message>
Add clusters.xlsx + Markowitz for the presentation
</commit_message>
<xml_diff>
--- a/clusters.xlsx
+++ b/clusters.xlsx
@@ -1773,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1784,7 +1784,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1817,7 +1817,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1839,7 +1839,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1850,7 +1850,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1861,7 +1861,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1872,7 +1872,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1883,7 +1883,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1894,7 +1894,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1905,7 +1905,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1927,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1938,7 +1938,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1960,7 +1960,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1971,7 +1971,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1993,7 +1993,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2004,7 +2004,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2026,7 +2026,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2037,7 +2037,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2059,7 +2059,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2070,7 +2070,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2081,7 +2081,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2092,7 +2092,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2103,7 +2103,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2114,7 +2114,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2125,7 +2125,7 @@
         <v>34</v>
       </c>
       <c r="C34">
-        <v>78</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2136,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2147,7 +2147,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2158,7 +2158,7 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2169,7 +2169,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2180,7 +2180,7 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2191,7 +2191,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2202,7 +2202,7 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2213,7 +2213,7 @@
         <v>42</v>
       </c>
       <c r="C42">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2224,7 +2224,7 @@
         <v>43</v>
       </c>
       <c r="C43">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2235,7 +2235,7 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2246,7 +2246,7 @@
         <v>45</v>
       </c>
       <c r="C45">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2257,7 +2257,7 @@
         <v>46</v>
       </c>
       <c r="C46">
-        <v>76</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2268,7 +2268,7 @@
         <v>47</v>
       </c>
       <c r="C47">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2279,7 +2279,7 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2290,7 +2290,7 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2301,7 +2301,7 @@
         <v>50</v>
       </c>
       <c r="C50">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2312,7 +2312,7 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2323,7 +2323,7 @@
         <v>52</v>
       </c>
       <c r="C52">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2345,7 +2345,7 @@
         <v>54</v>
       </c>
       <c r="C54">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2356,7 +2356,7 @@
         <v>55</v>
       </c>
       <c r="C55">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2367,7 +2367,7 @@
         <v>56</v>
       </c>
       <c r="C56">
-        <v>77</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2378,7 +2378,7 @@
         <v>57</v>
       </c>
       <c r="C57">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2389,7 +2389,7 @@
         <v>58</v>
       </c>
       <c r="C58">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2400,7 +2400,7 @@
         <v>59</v>
       </c>
       <c r="C59">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2411,7 +2411,7 @@
         <v>60</v>
       </c>
       <c r="C60">
-        <v>50</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2422,7 +2422,7 @@
         <v>61</v>
       </c>
       <c r="C61">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2433,7 +2433,7 @@
         <v>62</v>
       </c>
       <c r="C62">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2444,7 +2444,7 @@
         <v>63</v>
       </c>
       <c r="C63">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2455,7 +2455,7 @@
         <v>64</v>
       </c>
       <c r="C64">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2466,7 +2466,7 @@
         <v>65</v>
       </c>
       <c r="C65">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2477,7 +2477,7 @@
         <v>66</v>
       </c>
       <c r="C66">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2488,7 +2488,7 @@
         <v>67</v>
       </c>
       <c r="C67">
-        <v>83</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2499,7 +2499,7 @@
         <v>68</v>
       </c>
       <c r="C68">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2510,7 +2510,7 @@
         <v>69</v>
       </c>
       <c r="C69">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2521,7 +2521,7 @@
         <v>70</v>
       </c>
       <c r="C70">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2565,7 +2565,7 @@
         <v>74</v>
       </c>
       <c r="C74">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2587,7 +2587,7 @@
         <v>76</v>
       </c>
       <c r="C76">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2598,7 +2598,7 @@
         <v>77</v>
       </c>
       <c r="C77">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2609,7 +2609,7 @@
         <v>78</v>
       </c>
       <c r="C78">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2642,7 +2642,7 @@
         <v>81</v>
       </c>
       <c r="C81">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2664,7 +2664,7 @@
         <v>83</v>
       </c>
       <c r="C83">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2675,7 +2675,7 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>30</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2686,7 +2686,7 @@
         <v>85</v>
       </c>
       <c r="C85">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2697,7 +2697,7 @@
         <v>86</v>
       </c>
       <c r="C86">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2708,7 +2708,7 @@
         <v>87</v>
       </c>
       <c r="C87">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2719,7 +2719,7 @@
         <v>88</v>
       </c>
       <c r="C88">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2730,7 +2730,7 @@
         <v>89</v>
       </c>
       <c r="C89">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2741,7 +2741,7 @@
         <v>90</v>
       </c>
       <c r="C90">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2752,7 +2752,7 @@
         <v>91</v>
       </c>
       <c r="C91">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2763,7 +2763,7 @@
         <v>92</v>
       </c>
       <c r="C92">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2785,7 +2785,7 @@
         <v>94</v>
       </c>
       <c r="C94">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2796,7 +2796,7 @@
         <v>95</v>
       </c>
       <c r="C95">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2807,7 +2807,7 @@
         <v>96</v>
       </c>
       <c r="C96">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2818,7 +2818,7 @@
         <v>97</v>
       </c>
       <c r="C97">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2829,7 +2829,7 @@
         <v>98</v>
       </c>
       <c r="C98">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2840,7 +2840,7 @@
         <v>99</v>
       </c>
       <c r="C99">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2851,7 +2851,7 @@
         <v>100</v>
       </c>
       <c r="C100">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2862,7 +2862,7 @@
         <v>101</v>
       </c>
       <c r="C101">
-        <v>93</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2884,7 +2884,7 @@
         <v>103</v>
       </c>
       <c r="C103">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2895,7 +2895,7 @@
         <v>104</v>
       </c>
       <c r="C104">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2906,7 +2906,7 @@
         <v>105</v>
       </c>
       <c r="C105">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2917,7 +2917,7 @@
         <v>106</v>
       </c>
       <c r="C106">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2928,7 +2928,7 @@
         <v>107</v>
       </c>
       <c r="C107">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2939,7 +2939,7 @@
         <v>108</v>
       </c>
       <c r="C108">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2950,7 +2950,7 @@
         <v>109</v>
       </c>
       <c r="C109">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2961,7 +2961,7 @@
         <v>110</v>
       </c>
       <c r="C110">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2972,7 +2972,7 @@
         <v>111</v>
       </c>
       <c r="C111">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2983,7 +2983,7 @@
         <v>112</v>
       </c>
       <c r="C112">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2994,7 +2994,7 @@
         <v>113</v>
       </c>
       <c r="C113">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3005,7 +3005,7 @@
         <v>114</v>
       </c>
       <c r="C114">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3016,7 +3016,7 @@
         <v>115</v>
       </c>
       <c r="C115">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3027,7 +3027,7 @@
         <v>116</v>
       </c>
       <c r="C116">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3038,7 +3038,7 @@
         <v>117</v>
       </c>
       <c r="C117">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3049,7 +3049,7 @@
         <v>118</v>
       </c>
       <c r="C118">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3060,7 +3060,7 @@
         <v>119</v>
       </c>
       <c r="C119">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3071,7 +3071,7 @@
         <v>120</v>
       </c>
       <c r="C120">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -3082,7 +3082,7 @@
         <v>121</v>
       </c>
       <c r="C121">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3093,7 +3093,7 @@
         <v>122</v>
       </c>
       <c r="C122">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3104,7 +3104,7 @@
         <v>123</v>
       </c>
       <c r="C123">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3115,7 +3115,7 @@
         <v>124</v>
       </c>
       <c r="C124">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3126,7 +3126,7 @@
         <v>125</v>
       </c>
       <c r="C125">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3137,7 +3137,7 @@
         <v>126</v>
       </c>
       <c r="C126">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3148,7 +3148,7 @@
         <v>127</v>
       </c>
       <c r="C127">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -3159,7 +3159,7 @@
         <v>128</v>
       </c>
       <c r="C128">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3170,7 +3170,7 @@
         <v>129</v>
       </c>
       <c r="C129">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -3181,7 +3181,7 @@
         <v>130</v>
       </c>
       <c r="C130">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3192,7 +3192,7 @@
         <v>131</v>
       </c>
       <c r="C131">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3214,7 +3214,7 @@
         <v>133</v>
       </c>
       <c r="C133">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -3225,7 +3225,7 @@
         <v>134</v>
       </c>
       <c r="C134">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3236,7 +3236,7 @@
         <v>135</v>
       </c>
       <c r="C135">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -3247,7 +3247,7 @@
         <v>136</v>
       </c>
       <c r="C136">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3258,7 +3258,7 @@
         <v>137</v>
       </c>
       <c r="C137">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3269,7 +3269,7 @@
         <v>138</v>
       </c>
       <c r="C138">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3280,7 +3280,7 @@
         <v>139</v>
       </c>
       <c r="C139">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -3291,7 +3291,7 @@
         <v>140</v>
       </c>
       <c r="C140">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3302,7 +3302,7 @@
         <v>141</v>
       </c>
       <c r="C141">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3313,7 +3313,7 @@
         <v>142</v>
       </c>
       <c r="C142">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -3324,7 +3324,7 @@
         <v>143</v>
       </c>
       <c r="C143">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -3335,7 +3335,7 @@
         <v>144</v>
       </c>
       <c r="C144">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3346,7 +3346,7 @@
         <v>145</v>
       </c>
       <c r="C145">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3357,7 +3357,7 @@
         <v>146</v>
       </c>
       <c r="C146">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3368,7 +3368,7 @@
         <v>147</v>
       </c>
       <c r="C147">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3379,7 +3379,7 @@
         <v>148</v>
       </c>
       <c r="C148">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3390,7 +3390,7 @@
         <v>149</v>
       </c>
       <c r="C149">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3401,7 +3401,7 @@
         <v>150</v>
       </c>
       <c r="C150">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3412,7 +3412,7 @@
         <v>151</v>
       </c>
       <c r="C151">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3423,7 +3423,7 @@
         <v>152</v>
       </c>
       <c r="C152">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3434,7 +3434,7 @@
         <v>153</v>
       </c>
       <c r="C153">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3445,7 +3445,7 @@
         <v>154</v>
       </c>
       <c r="C154">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3456,7 +3456,7 @@
         <v>155</v>
       </c>
       <c r="C155">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3467,7 +3467,7 @@
         <v>156</v>
       </c>
       <c r="C156">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3478,7 +3478,7 @@
         <v>157</v>
       </c>
       <c r="C157">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3489,7 +3489,7 @@
         <v>158</v>
       </c>
       <c r="C158">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3500,7 +3500,7 @@
         <v>159</v>
       </c>
       <c r="C159">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3511,7 +3511,7 @@
         <v>160</v>
       </c>
       <c r="C160">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3522,7 +3522,7 @@
         <v>161</v>
       </c>
       <c r="C161">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3533,7 +3533,7 @@
         <v>162</v>
       </c>
       <c r="C162">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3555,7 +3555,7 @@
         <v>164</v>
       </c>
       <c r="C164">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3566,7 +3566,7 @@
         <v>165</v>
       </c>
       <c r="C165">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3577,7 +3577,7 @@
         <v>166</v>
       </c>
       <c r="C166">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3588,7 +3588,7 @@
         <v>167</v>
       </c>
       <c r="C167">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3599,7 +3599,7 @@
         <v>168</v>
       </c>
       <c r="C168">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3610,7 +3610,7 @@
         <v>169</v>
       </c>
       <c r="C169">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3621,7 +3621,7 @@
         <v>170</v>
       </c>
       <c r="C170">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3632,7 +3632,7 @@
         <v>171</v>
       </c>
       <c r="C171">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3643,7 +3643,7 @@
         <v>172</v>
       </c>
       <c r="C172">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3654,7 +3654,7 @@
         <v>173</v>
       </c>
       <c r="C173">
-        <v>50</v>
+        <v>106</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3665,7 +3665,7 @@
         <v>174</v>
       </c>
       <c r="C174">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3676,7 +3676,7 @@
         <v>175</v>
       </c>
       <c r="C175">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3687,7 +3687,7 @@
         <v>176</v>
       </c>
       <c r="C176">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3698,7 +3698,7 @@
         <v>177</v>
       </c>
       <c r="C177">
-        <v>79</v>
+        <v>34</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3720,7 +3720,7 @@
         <v>179</v>
       </c>
       <c r="C179">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3731,7 +3731,7 @@
         <v>180</v>
       </c>
       <c r="C180">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3742,7 +3742,7 @@
         <v>181</v>
       </c>
       <c r="C181">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3753,7 +3753,7 @@
         <v>182</v>
       </c>
       <c r="C182">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3764,7 +3764,7 @@
         <v>183</v>
       </c>
       <c r="C183">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3775,7 +3775,7 @@
         <v>184</v>
       </c>
       <c r="C184">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3786,7 +3786,7 @@
         <v>185</v>
       </c>
       <c r="C185">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3797,7 +3797,7 @@
         <v>186</v>
       </c>
       <c r="C186">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3808,7 +3808,7 @@
         <v>187</v>
       </c>
       <c r="C187">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3819,7 +3819,7 @@
         <v>188</v>
       </c>
       <c r="C188">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3830,7 +3830,7 @@
         <v>189</v>
       </c>
       <c r="C189">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3841,7 +3841,7 @@
         <v>190</v>
       </c>
       <c r="C190">
-        <v>18</v>
+        <v>110</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3852,7 +3852,7 @@
         <v>191</v>
       </c>
       <c r="C191">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3863,7 +3863,7 @@
         <v>192</v>
       </c>
       <c r="C192">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3874,7 +3874,7 @@
         <v>193</v>
       </c>
       <c r="C193">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3885,7 +3885,7 @@
         <v>194</v>
       </c>
       <c r="C194">
-        <v>99</v>
+        <v>23</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3896,7 +3896,7 @@
         <v>195</v>
       </c>
       <c r="C195">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3907,7 +3907,7 @@
         <v>196</v>
       </c>
       <c r="C196">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3918,7 +3918,7 @@
         <v>197</v>
       </c>
       <c r="C197">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3929,7 +3929,7 @@
         <v>198</v>
       </c>
       <c r="C198">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3940,7 +3940,7 @@
         <v>199</v>
       </c>
       <c r="C199">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3951,7 +3951,7 @@
         <v>200</v>
       </c>
       <c r="C200">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3962,7 +3962,7 @@
         <v>201</v>
       </c>
       <c r="C201">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3973,7 +3973,7 @@
         <v>202</v>
       </c>
       <c r="C202">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3984,7 +3984,7 @@
         <v>203</v>
       </c>
       <c r="C203">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3995,7 +3995,7 @@
         <v>204</v>
       </c>
       <c r="C204">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -4006,7 +4006,7 @@
         <v>205</v>
       </c>
       <c r="C205">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -4017,7 +4017,7 @@
         <v>206</v>
       </c>
       <c r="C206">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4028,7 +4028,7 @@
         <v>207</v>
       </c>
       <c r="C207">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -4039,7 +4039,7 @@
         <v>208</v>
       </c>
       <c r="C208">
-        <v>77</v>
+        <v>19</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -4050,7 +4050,7 @@
         <v>209</v>
       </c>
       <c r="C209">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -4061,7 +4061,7 @@
         <v>210</v>
       </c>
       <c r="C210">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -4083,7 +4083,7 @@
         <v>212</v>
       </c>
       <c r="C212">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -4094,7 +4094,7 @@
         <v>213</v>
       </c>
       <c r="C213">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -4105,7 +4105,7 @@
         <v>214</v>
       </c>
       <c r="C214">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -4116,7 +4116,7 @@
         <v>215</v>
       </c>
       <c r="C215">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -4127,7 +4127,7 @@
         <v>216</v>
       </c>
       <c r="C216">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -4149,7 +4149,7 @@
         <v>218</v>
       </c>
       <c r="C218">
-        <v>16</v>
+        <v>58</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -4160,7 +4160,7 @@
         <v>219</v>
       </c>
       <c r="C219">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -4171,7 +4171,7 @@
         <v>220</v>
       </c>
       <c r="C220">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -4182,7 +4182,7 @@
         <v>221</v>
       </c>
       <c r="C221">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -4204,7 +4204,7 @@
         <v>223</v>
       </c>
       <c r="C223">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -4215,7 +4215,7 @@
         <v>224</v>
       </c>
       <c r="C224">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -4226,7 +4226,7 @@
         <v>225</v>
       </c>
       <c r="C225">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -4237,7 +4237,7 @@
         <v>226</v>
       </c>
       <c r="C226">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -4248,7 +4248,7 @@
         <v>227</v>
       </c>
       <c r="C227">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -4259,7 +4259,7 @@
         <v>228</v>
       </c>
       <c r="C228">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -4270,7 +4270,7 @@
         <v>229</v>
       </c>
       <c r="C229">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -4281,7 +4281,7 @@
         <v>230</v>
       </c>
       <c r="C230">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -4292,7 +4292,7 @@
         <v>231</v>
       </c>
       <c r="C231">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -4303,7 +4303,7 @@
         <v>232</v>
       </c>
       <c r="C232">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -4314,7 +4314,7 @@
         <v>233</v>
       </c>
       <c r="C233">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -4325,7 +4325,7 @@
         <v>234</v>
       </c>
       <c r="C234">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -4336,7 +4336,7 @@
         <v>235</v>
       </c>
       <c r="C235">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -4347,7 +4347,7 @@
         <v>236</v>
       </c>
       <c r="C236">
-        <v>107</v>
+        <v>23</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -4358,7 +4358,7 @@
         <v>237</v>
       </c>
       <c r="C237">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -4369,7 +4369,7 @@
         <v>238</v>
       </c>
       <c r="C238">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -4380,7 +4380,7 @@
         <v>239</v>
       </c>
       <c r="C239">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -4391,7 +4391,7 @@
         <v>240</v>
       </c>
       <c r="C240">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -4402,7 +4402,7 @@
         <v>241</v>
       </c>
       <c r="C241">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -4413,7 +4413,7 @@
         <v>242</v>
       </c>
       <c r="C242">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -4435,7 +4435,7 @@
         <v>244</v>
       </c>
       <c r="C244">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -4446,7 +4446,7 @@
         <v>245</v>
       </c>
       <c r="C245">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -4457,7 +4457,7 @@
         <v>246</v>
       </c>
       <c r="C246">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -4468,7 +4468,7 @@
         <v>247</v>
       </c>
       <c r="C247">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -4479,7 +4479,7 @@
         <v>248</v>
       </c>
       <c r="C248">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -4490,7 +4490,7 @@
         <v>249</v>
       </c>
       <c r="C249">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -4501,7 +4501,7 @@
         <v>250</v>
       </c>
       <c r="C250">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -4512,7 +4512,7 @@
         <v>251</v>
       </c>
       <c r="C251">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -4523,7 +4523,7 @@
         <v>252</v>
       </c>
       <c r="C252">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -4534,7 +4534,7 @@
         <v>253</v>
       </c>
       <c r="C253">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -4545,7 +4545,7 @@
         <v>254</v>
       </c>
       <c r="C254">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -4556,7 +4556,7 @@
         <v>255</v>
       </c>
       <c r="C255">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -4567,7 +4567,7 @@
         <v>256</v>
       </c>
       <c r="C256">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4578,7 +4578,7 @@
         <v>257</v>
       </c>
       <c r="C257">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4589,7 +4589,7 @@
         <v>258</v>
       </c>
       <c r="C258">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4600,7 +4600,7 @@
         <v>259</v>
       </c>
       <c r="C259">
-        <v>110</v>
+        <v>67</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4611,7 +4611,7 @@
         <v>260</v>
       </c>
       <c r="C260">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4622,7 +4622,7 @@
         <v>261</v>
       </c>
       <c r="C261">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4633,7 +4633,7 @@
         <v>262</v>
       </c>
       <c r="C262">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4644,7 +4644,7 @@
         <v>263</v>
       </c>
       <c r="C263">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4655,7 +4655,7 @@
         <v>264</v>
       </c>
       <c r="C264">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4666,7 +4666,7 @@
         <v>265</v>
       </c>
       <c r="C265">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4677,7 +4677,7 @@
         <v>266</v>
       </c>
       <c r="C266">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4688,7 +4688,7 @@
         <v>267</v>
       </c>
       <c r="C267">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4699,7 +4699,7 @@
         <v>268</v>
       </c>
       <c r="C268">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4710,7 +4710,7 @@
         <v>269</v>
       </c>
       <c r="C269">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4721,7 +4721,7 @@
         <v>270</v>
       </c>
       <c r="C270">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4743,7 +4743,7 @@
         <v>272</v>
       </c>
       <c r="C272">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -4754,7 +4754,7 @@
         <v>273</v>
       </c>
       <c r="C273">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -4765,7 +4765,7 @@
         <v>274</v>
       </c>
       <c r="C274">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -4776,7 +4776,7 @@
         <v>275</v>
       </c>
       <c r="C275">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -4787,7 +4787,7 @@
         <v>276</v>
       </c>
       <c r="C276">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -4798,7 +4798,7 @@
         <v>277</v>
       </c>
       <c r="C277">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -4809,7 +4809,7 @@
         <v>278</v>
       </c>
       <c r="C278">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -4820,7 +4820,7 @@
         <v>279</v>
       </c>
       <c r="C279">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -4831,7 +4831,7 @@
         <v>280</v>
       </c>
       <c r="C280">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -4842,7 +4842,7 @@
         <v>281</v>
       </c>
       <c r="C281">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -4853,7 +4853,7 @@
         <v>282</v>
       </c>
       <c r="C282">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -4864,7 +4864,7 @@
         <v>283</v>
       </c>
       <c r="C283">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -4875,7 +4875,7 @@
         <v>284</v>
       </c>
       <c r="C284">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -4886,7 +4886,7 @@
         <v>285</v>
       </c>
       <c r="C285">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="286" spans="1:3">
@@ -4897,7 +4897,7 @@
         <v>286</v>
       </c>
       <c r="C286">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -4908,7 +4908,7 @@
         <v>287</v>
       </c>
       <c r="C287">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4919,7 +4919,7 @@
         <v>288</v>
       </c>
       <c r="C288">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="289" spans="1:3">
@@ -4930,7 +4930,7 @@
         <v>289</v>
       </c>
       <c r="C289">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="290" spans="1:3">
@@ -4941,7 +4941,7 @@
         <v>290</v>
       </c>
       <c r="C290">
-        <v>107</v>
+        <v>71</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -4952,7 +4952,7 @@
         <v>291</v>
       </c>
       <c r="C291">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -4963,7 +4963,7 @@
         <v>292</v>
       </c>
       <c r="C292">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="293" spans="1:3">
@@ -4974,7 +4974,7 @@
         <v>293</v>
       </c>
       <c r="C293">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -4985,7 +4985,7 @@
         <v>294</v>
       </c>
       <c r="C294">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -4996,7 +4996,7 @@
         <v>295</v>
       </c>
       <c r="C295">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="296" spans="1:3">
@@ -5007,7 +5007,7 @@
         <v>296</v>
       </c>
       <c r="C296">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -5018,7 +5018,7 @@
         <v>297</v>
       </c>
       <c r="C297">
-        <v>83</v>
+        <v>43</v>
       </c>
     </row>
     <row r="298" spans="1:3">
@@ -5029,7 +5029,7 @@
         <v>298</v>
       </c>
       <c r="C298">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="299" spans="1:3">
@@ -5040,7 +5040,7 @@
         <v>299</v>
       </c>
       <c r="C299">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="300" spans="1:3">
@@ -5051,7 +5051,7 @@
         <v>300</v>
       </c>
       <c r="C300">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="301" spans="1:3">
@@ -5073,7 +5073,7 @@
         <v>302</v>
       </c>
       <c r="C302">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="303" spans="1:3">
@@ -5084,7 +5084,7 @@
         <v>303</v>
       </c>
       <c r="C303">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="304" spans="1:3">
@@ -5095,7 +5095,7 @@
         <v>304</v>
       </c>
       <c r="C304">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="305" spans="1:3">
@@ -5117,7 +5117,7 @@
         <v>306</v>
       </c>
       <c r="C306">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -5128,7 +5128,7 @@
         <v>307</v>
       </c>
       <c r="C307">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="308" spans="1:3">
@@ -5139,7 +5139,7 @@
         <v>308</v>
       </c>
       <c r="C308">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="309" spans="1:3">
@@ -5150,7 +5150,7 @@
         <v>309</v>
       </c>
       <c r="C309">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="310" spans="1:3">
@@ -5161,7 +5161,7 @@
         <v>310</v>
       </c>
       <c r="C310">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -5172,7 +5172,7 @@
         <v>311</v>
       </c>
       <c r="C311">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="312" spans="1:3">
@@ -5183,7 +5183,7 @@
         <v>312</v>
       </c>
       <c r="C312">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="313" spans="1:3">
@@ -5194,7 +5194,7 @@
         <v>313</v>
       </c>
       <c r="C313">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -5205,7 +5205,7 @@
         <v>314</v>
       </c>
       <c r="C314">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="315" spans="1:3">
@@ -5216,7 +5216,7 @@
         <v>315</v>
       </c>
       <c r="C315">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="316" spans="1:3">
@@ -5227,7 +5227,7 @@
         <v>316</v>
       </c>
       <c r="C316">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="317" spans="1:3">
@@ -5249,7 +5249,7 @@
         <v>318</v>
       </c>
       <c r="C318">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="319" spans="1:3">
@@ -5260,7 +5260,7 @@
         <v>319</v>
       </c>
       <c r="C319">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="320" spans="1:3">
@@ -5271,7 +5271,7 @@
         <v>320</v>
       </c>
       <c r="C320">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="321" spans="1:3">
@@ -5282,7 +5282,7 @@
         <v>321</v>
       </c>
       <c r="C321">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="322" spans="1:3">
@@ -5293,7 +5293,7 @@
         <v>322</v>
       </c>
       <c r="C322">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -5304,7 +5304,7 @@
         <v>323</v>
       </c>
       <c r="C323">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="324" spans="1:3">
@@ -5315,7 +5315,7 @@
         <v>324</v>
       </c>
       <c r="C324">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="325" spans="1:3">
@@ -5326,7 +5326,7 @@
         <v>325</v>
       </c>
       <c r="C325">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -5337,7 +5337,7 @@
         <v>326</v>
       </c>
       <c r="C326">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -5348,7 +5348,7 @@
         <v>327</v>
       </c>
       <c r="C327">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="328" spans="1:3">
@@ -5359,7 +5359,7 @@
         <v>328</v>
       </c>
       <c r="C328">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="329" spans="1:3">
@@ -5370,7 +5370,7 @@
         <v>329</v>
       </c>
       <c r="C329">
-        <v>83</v>
+        <v>22</v>
       </c>
     </row>
     <row r="330" spans="1:3">
@@ -5381,7 +5381,7 @@
         <v>330</v>
       </c>
       <c r="C330">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -5403,7 +5403,7 @@
         <v>332</v>
       </c>
       <c r="C332">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="333" spans="1:3">
@@ -5414,7 +5414,7 @@
         <v>333</v>
       </c>
       <c r="C333">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="334" spans="1:3">
@@ -5425,7 +5425,7 @@
         <v>334</v>
       </c>
       <c r="C334">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -5436,7 +5436,7 @@
         <v>335</v>
       </c>
       <c r="C335">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -5447,7 +5447,7 @@
         <v>336</v>
       </c>
       <c r="C336">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="337" spans="1:3">
@@ -5458,7 +5458,7 @@
         <v>337</v>
       </c>
       <c r="C337">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -5469,7 +5469,7 @@
         <v>338</v>
       </c>
       <c r="C338">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -5480,7 +5480,7 @@
         <v>339</v>
       </c>
       <c r="C339">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="340" spans="1:3">
@@ -5491,7 +5491,7 @@
         <v>340</v>
       </c>
       <c r="C340">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -5502,7 +5502,7 @@
         <v>341</v>
       </c>
       <c r="C341">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="342" spans="1:3">
@@ -5513,7 +5513,7 @@
         <v>342</v>
       </c>
       <c r="C342">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -5524,7 +5524,7 @@
         <v>343</v>
       </c>
       <c r="C343">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -5535,7 +5535,7 @@
         <v>344</v>
       </c>
       <c r="C344">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -5546,7 +5546,7 @@
         <v>345</v>
       </c>
       <c r="C345">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="346" spans="1:3">
@@ -5557,7 +5557,7 @@
         <v>346</v>
       </c>
       <c r="C346">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="347" spans="1:3">
@@ -5568,7 +5568,7 @@
         <v>347</v>
       </c>
       <c r="C347">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="348" spans="1:3">
@@ -5579,7 +5579,7 @@
         <v>348</v>
       </c>
       <c r="C348">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="349" spans="1:3">
@@ -5590,7 +5590,7 @@
         <v>349</v>
       </c>
       <c r="C349">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="350" spans="1:3">
@@ -5601,7 +5601,7 @@
         <v>350</v>
       </c>
       <c r="C350">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -5612,7 +5612,7 @@
         <v>351</v>
       </c>
       <c r="C351">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="352" spans="1:3">
@@ -5623,7 +5623,7 @@
         <v>352</v>
       </c>
       <c r="C352">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="353" spans="1:3">
@@ -5634,7 +5634,7 @@
         <v>353</v>
       </c>
       <c r="C353">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="354" spans="1:3">
@@ -5645,7 +5645,7 @@
         <v>354</v>
       </c>
       <c r="C354">
-        <v>22</v>
+        <v>99</v>
       </c>
     </row>
     <row r="355" spans="1:3">
@@ -5656,7 +5656,7 @@
         <v>355</v>
       </c>
       <c r="C355">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="356" spans="1:3">
@@ -5667,7 +5667,7 @@
         <v>356</v>
       </c>
       <c r="C356">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="357" spans="1:3">
@@ -5678,7 +5678,7 @@
         <v>357</v>
       </c>
       <c r="C357">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="358" spans="1:3">
@@ -5689,7 +5689,7 @@
         <v>358</v>
       </c>
       <c r="C358">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="359" spans="1:3">
@@ -5711,7 +5711,7 @@
         <v>360</v>
       </c>
       <c r="C360">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="361" spans="1:3">
@@ -5722,7 +5722,7 @@
         <v>361</v>
       </c>
       <c r="C361">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="362" spans="1:3">
@@ -5733,7 +5733,7 @@
         <v>362</v>
       </c>
       <c r="C362">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="363" spans="1:3">
@@ -5744,7 +5744,7 @@
         <v>363</v>
       </c>
       <c r="C363">
-        <v>105</v>
+        <v>68</v>
       </c>
     </row>
     <row r="364" spans="1:3">
@@ -5755,7 +5755,7 @@
         <v>364</v>
       </c>
       <c r="C364">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="365" spans="1:3">
@@ -5766,7 +5766,7 @@
         <v>365</v>
       </c>
       <c r="C365">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="366" spans="1:3">
@@ -5788,7 +5788,7 @@
         <v>367</v>
       </c>
       <c r="C367">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="368" spans="1:3">
@@ -5799,7 +5799,7 @@
         <v>368</v>
       </c>
       <c r="C368">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="369" spans="1:3">
@@ -5810,7 +5810,7 @@
         <v>369</v>
       </c>
       <c r="C369">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="370" spans="1:3">
@@ -5821,7 +5821,7 @@
         <v>370</v>
       </c>
       <c r="C370">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="371" spans="1:3">
@@ -5832,7 +5832,7 @@
         <v>371</v>
       </c>
       <c r="C371">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="372" spans="1:3">
@@ -5843,7 +5843,7 @@
         <v>372</v>
       </c>
       <c r="C372">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="373" spans="1:3">
@@ -5854,7 +5854,7 @@
         <v>373</v>
       </c>
       <c r="C373">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="374" spans="1:3">
@@ -5865,7 +5865,7 @@
         <v>374</v>
       </c>
       <c r="C374">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="375" spans="1:3">
@@ -5876,7 +5876,7 @@
         <v>375</v>
       </c>
       <c r="C375">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="376" spans="1:3">
@@ -5887,7 +5887,7 @@
         <v>376</v>
       </c>
       <c r="C376">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="377" spans="1:3">
@@ -5898,7 +5898,7 @@
         <v>377</v>
       </c>
       <c r="C377">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="378" spans="1:3">
@@ -5909,7 +5909,7 @@
         <v>378</v>
       </c>
       <c r="C378">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="379" spans="1:3">
@@ -5920,7 +5920,7 @@
         <v>379</v>
       </c>
       <c r="C379">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -5931,7 +5931,7 @@
         <v>380</v>
       </c>
       <c r="C380">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -5942,7 +5942,7 @@
         <v>381</v>
       </c>
       <c r="C381">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="382" spans="1:3">
@@ -5953,7 +5953,7 @@
         <v>382</v>
       </c>
       <c r="C382">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="383" spans="1:3">
@@ -5964,7 +5964,7 @@
         <v>383</v>
       </c>
       <c r="C383">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="384" spans="1:3">
@@ -5975,7 +5975,7 @@
         <v>384</v>
       </c>
       <c r="C384">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -5986,7 +5986,7 @@
         <v>385</v>
       </c>
       <c r="C385">
-        <v>30</v>
+        <v>102</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -5997,7 +5997,7 @@
         <v>386</v>
       </c>
       <c r="C386">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="387" spans="1:3">
@@ -6008,7 +6008,7 @@
         <v>387</v>
       </c>
       <c r="C387">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -6019,7 +6019,7 @@
         <v>388</v>
       </c>
       <c r="C388">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -6030,7 +6030,7 @@
         <v>389</v>
       </c>
       <c r="C389">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="390" spans="1:3">
@@ -6041,7 +6041,7 @@
         <v>390</v>
       </c>
       <c r="C390">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="391" spans="1:3">
@@ -6052,7 +6052,7 @@
         <v>391</v>
       </c>
       <c r="C391">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="392" spans="1:3">
@@ -6063,7 +6063,7 @@
         <v>392</v>
       </c>
       <c r="C392">
-        <v>3</v>
+        <v>114</v>
       </c>
     </row>
     <row r="393" spans="1:3">
@@ -6074,7 +6074,7 @@
         <v>393</v>
       </c>
       <c r="C393">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="394" spans="1:3">
@@ -6085,7 +6085,7 @@
         <v>394</v>
       </c>
       <c r="C394">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="395" spans="1:3">
@@ -6096,7 +6096,7 @@
         <v>395</v>
       </c>
       <c r="C395">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="396" spans="1:3">
@@ -6107,7 +6107,7 @@
         <v>396</v>
       </c>
       <c r="C396">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="397" spans="1:3">
@@ -6118,7 +6118,7 @@
         <v>397</v>
       </c>
       <c r="C397">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="398" spans="1:3">
@@ -6129,7 +6129,7 @@
         <v>398</v>
       </c>
       <c r="C398">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="399" spans="1:3">
@@ -6140,7 +6140,7 @@
         <v>399</v>
       </c>
       <c r="C399">
-        <v>37</v>
+        <v>103</v>
       </c>
     </row>
     <row r="400" spans="1:3">
@@ -6151,7 +6151,7 @@
         <v>400</v>
       </c>
       <c r="C400">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="401" spans="1:3">
@@ -6162,7 +6162,7 @@
         <v>401</v>
       </c>
       <c r="C401">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="402" spans="1:3">
@@ -6173,7 +6173,7 @@
         <v>402</v>
       </c>
       <c r="C402">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="403" spans="1:3">
@@ -6184,7 +6184,7 @@
         <v>403</v>
       </c>
       <c r="C403">
-        <v>54</v>
+        <v>103</v>
       </c>
     </row>
     <row r="404" spans="1:3">
@@ -6195,7 +6195,7 @@
         <v>404</v>
       </c>
       <c r="C404">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="405" spans="1:3">
@@ -6217,7 +6217,7 @@
         <v>406</v>
       </c>
       <c r="C406">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="407" spans="1:3">
@@ -6228,7 +6228,7 @@
         <v>407</v>
       </c>
       <c r="C407">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="408" spans="1:3">
@@ -6239,7 +6239,7 @@
         <v>408</v>
       </c>
       <c r="C408">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="409" spans="1:3">
@@ -6250,7 +6250,7 @@
         <v>409</v>
       </c>
       <c r="C409">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="410" spans="1:3">
@@ -6261,7 +6261,7 @@
         <v>410</v>
       </c>
       <c r="C410">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="411" spans="1:3">
@@ -6272,7 +6272,7 @@
         <v>411</v>
       </c>
       <c r="C411">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="412" spans="1:3">
@@ -6283,7 +6283,7 @@
         <v>412</v>
       </c>
       <c r="C412">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -6294,7 +6294,7 @@
         <v>413</v>
       </c>
       <c r="C413">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="414" spans="1:3">
@@ -6305,7 +6305,7 @@
         <v>414</v>
       </c>
       <c r="C414">
-        <v>17</v>
+        <v>102</v>
       </c>
     </row>
     <row r="415" spans="1:3">
@@ -6316,7 +6316,7 @@
         <v>415</v>
       </c>
       <c r="C415">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="416" spans="1:3">
@@ -6327,7 +6327,7 @@
         <v>416</v>
       </c>
       <c r="C416">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="417" spans="1:3">
@@ -6338,7 +6338,7 @@
         <v>417</v>
       </c>
       <c r="C417">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
     <row r="418" spans="1:3">
@@ -6360,7 +6360,7 @@
         <v>419</v>
       </c>
       <c r="C419">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="420" spans="1:3">
@@ -6371,7 +6371,7 @@
         <v>420</v>
       </c>
       <c r="C420">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="421" spans="1:3">
@@ -6382,7 +6382,7 @@
         <v>421</v>
       </c>
       <c r="C421">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="422" spans="1:3">
@@ -6393,7 +6393,7 @@
         <v>422</v>
       </c>
       <c r="C422">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="423" spans="1:3">
@@ -6404,7 +6404,7 @@
         <v>423</v>
       </c>
       <c r="C423">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="424" spans="1:3">
@@ -6415,7 +6415,7 @@
         <v>424</v>
       </c>
       <c r="C424">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="425" spans="1:3">
@@ -6426,7 +6426,7 @@
         <v>425</v>
       </c>
       <c r="C425">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="426" spans="1:3">
@@ -6437,7 +6437,7 @@
         <v>426</v>
       </c>
       <c r="C426">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -6448,7 +6448,7 @@
         <v>427</v>
       </c>
       <c r="C427">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="428" spans="1:3">
@@ -6459,7 +6459,7 @@
         <v>428</v>
       </c>
       <c r="C428">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="429" spans="1:3">
@@ -6470,7 +6470,7 @@
         <v>429</v>
       </c>
       <c r="C429">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="430" spans="1:3">
@@ -6492,7 +6492,7 @@
         <v>431</v>
       </c>
       <c r="C431">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="432" spans="1:3">
@@ -6503,7 +6503,7 @@
         <v>432</v>
       </c>
       <c r="C432">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="433" spans="1:3">
@@ -6514,7 +6514,7 @@
         <v>433</v>
       </c>
       <c r="C433">
-        <v>50</v>
+        <v>106</v>
       </c>
     </row>
     <row r="434" spans="1:3">
@@ -6525,7 +6525,7 @@
         <v>434</v>
       </c>
       <c r="C434">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="435" spans="1:3">
@@ -6536,7 +6536,7 @@
         <v>435</v>
       </c>
       <c r="C435">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="436" spans="1:3">
@@ -6547,7 +6547,7 @@
         <v>436</v>
       </c>
       <c r="C436">
-        <v>35</v>
+        <v>107</v>
       </c>
     </row>
     <row r="437" spans="1:3">
@@ -6569,7 +6569,7 @@
         <v>438</v>
       </c>
       <c r="C438">
-        <v>83</v>
+        <v>109</v>
       </c>
     </row>
     <row r="439" spans="1:3">
@@ -6580,7 +6580,7 @@
         <v>439</v>
       </c>
       <c r="C439">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="440" spans="1:3">
@@ -6591,7 +6591,7 @@
         <v>440</v>
       </c>
       <c r="C440">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="441" spans="1:3">
@@ -6602,7 +6602,7 @@
         <v>441</v>
       </c>
       <c r="C441">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="442" spans="1:3">
@@ -6613,7 +6613,7 @@
         <v>442</v>
       </c>
       <c r="C442">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="443" spans="1:3">
@@ -6624,7 +6624,7 @@
         <v>443</v>
       </c>
       <c r="C443">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="444" spans="1:3">
@@ -6635,7 +6635,7 @@
         <v>444</v>
       </c>
       <c r="C444">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="445" spans="1:3">
@@ -6646,7 +6646,7 @@
         <v>445</v>
       </c>
       <c r="C445">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="446" spans="1:3">
@@ -6657,7 +6657,7 @@
         <v>446</v>
       </c>
       <c r="C446">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="447" spans="1:3">
@@ -6668,7 +6668,7 @@
         <v>447</v>
       </c>
       <c r="C447">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="448" spans="1:3">
@@ -6679,7 +6679,7 @@
         <v>448</v>
       </c>
       <c r="C448">
-        <v>35</v>
+        <v>111</v>
       </c>
     </row>
     <row r="449" spans="1:3">
@@ -6690,7 +6690,7 @@
         <v>449</v>
       </c>
       <c r="C449">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="450" spans="1:3">
@@ -6701,7 +6701,7 @@
         <v>450</v>
       </c>
       <c r="C450">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="451" spans="1:3">
@@ -6712,7 +6712,7 @@
         <v>451</v>
       </c>
       <c r="C451">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="452" spans="1:3">
@@ -6723,7 +6723,7 @@
         <v>452</v>
       </c>
       <c r="C452">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="453" spans="1:3">
@@ -6734,7 +6734,7 @@
         <v>453</v>
       </c>
       <c r="C453">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="454" spans="1:3">
@@ -6745,7 +6745,7 @@
         <v>454</v>
       </c>
       <c r="C454">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="455" spans="1:3">
@@ -6756,7 +6756,7 @@
         <v>455</v>
       </c>
       <c r="C455">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="456" spans="1:3">
@@ -6767,7 +6767,7 @@
         <v>456</v>
       </c>
       <c r="C456">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="457" spans="1:3">
@@ -6778,7 +6778,7 @@
         <v>457</v>
       </c>
       <c r="C457">
-        <v>18</v>
+        <v>68</v>
       </c>
     </row>
     <row r="458" spans="1:3">
@@ -6789,7 +6789,7 @@
         <v>458</v>
       </c>
       <c r="C458">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="459" spans="1:3">
@@ -6800,7 +6800,7 @@
         <v>459</v>
       </c>
       <c r="C459">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>